<commit_message>
changed title of column
</commit_message>
<xml_diff>
--- a/zoom.xlsx
+++ b/zoom.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Password(Blank if no)</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t xml:space="preserve">Time To Join (Do Earlier than Start of Class)</t>
   </si>
   <si>
     <t xml:space="preserve">Monday</t>
@@ -55,10 +55,10 @@
     <t xml:space="preserve">Sunday</t>
   </si>
   <si>
-    <t xml:space="preserve">Start Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End Date</t>
+    <t xml:space="preserve">Class Start Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class End Date</t>
   </si>
 </sst>
 </file>
@@ -179,13 +179,16 @@
   <dimension ref="A1:M107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:M1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="106.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added funcitonality for creating a direct link to open zoom without opening browser
</commit_message>
<xml_diff>
--- a/zoom.xlsx
+++ b/zoom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Class Name</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t xml:space="preserve">Class End Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No App Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open application Link</t>
   </si>
 </sst>
 </file>
@@ -142,12 +148,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,10 +186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O:O"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -189,6 +199,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -231,16 +243,22 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1"/>
-      <c r="L2" s="2"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>